<commit_message>
Updated matlab codes for metamodeling with a relatively higher std-dev as compared to the prevous version
</commit_message>
<xml_diff>
--- a/data/072919-INS1e-30min-Enrichment-analysis-cleaned-summary.xlsx
+++ b/data/072919-INS1e-30min-Enrichment-analysis-cleaned-summary.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB9D6B6-003E-5547-8292-4E91684BD6C6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40896C0D-091E-6A45-94EC-DBE056EFEFBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="44">
   <si>
     <t>SIZE</t>
   </si>
@@ -121,72 +121,6 @@
     <t>High glucose +Ex4 vs high glucose -Ex4</t>
   </si>
   <si>
-    <t>High glucose +Ex4 vs high glucose -Ex5</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex6</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex7</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex8</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex9</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex10</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex11</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex12</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex13</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex14</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex15</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex16</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex17</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex18</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex19</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex20</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex21</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex22</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex23</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex24</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex25</t>
-  </si>
-  <si>
-    <t>High glucose +Ex4 vs high glucose -Ex26</t>
-  </si>
-  <si>
     <t>HG.vs.LG</t>
   </si>
   <si>
@@ -196,377 +130,38 @@
     <t>High glucose -Ex4 vs low glucose -Ex4</t>
   </si>
   <si>
-    <t>High glucose -Ex4 vs low glucose -Ex5</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex6</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex7</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex8</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex9</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex10</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex11</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex12</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex13</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex14</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex15</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex16</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex17</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex18</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex19</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex20</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex21</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex22</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex23</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex24</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs low glucose -Ex25</t>
-  </si>
-  <si>
     <t>HG.vs.MG</t>
   </si>
   <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex25</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex26</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex27</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex28</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex29</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex30</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex31</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex32</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex33</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex34</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex35</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex36</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex37</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex38</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex39</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex40</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex41</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex42</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex43</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex44</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex45</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex46</t>
-  </si>
-  <si>
-    <t>High glucose -Ex4 vs medium glucose -Ex47</t>
-  </si>
-  <si>
     <t>LG.pE.vs.mE</t>
   </si>
   <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex9</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex10</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex11</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex12</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex13</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex14</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex15</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex16</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex17</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex18</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex19</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex20</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex21</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex22</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex23</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex24</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex25</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex26</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex27</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex28</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex29</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex30</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex31</t>
-  </si>
-  <si>
-    <t>Low  glucose +Ex4 vs low glucose -Ex32</t>
-  </si>
-  <si>
     <t>MG.pE.vs.mE</t>
   </si>
   <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex32</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex33</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex34</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex35</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex36</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex37</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex38</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex39</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex40</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex41</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex42</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex43</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex44</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex45</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex46</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex47</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex48</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex49</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex50</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex51</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex52</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex53</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex54</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex55</t>
-  </si>
-  <si>
-    <t>Medium  glucose +Ex4 vs medium glucose -Ex56</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex17</t>
-  </si>
-  <si>
     <t>MG.vs.LG</t>
   </si>
   <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex18</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex19</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex20</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex21</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex22</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex23</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex24</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex25</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex26</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex27</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex28</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex29</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex30</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex31</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex32</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex33</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex34</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex35</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex36</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex37</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex38</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex39</t>
-  </si>
-  <si>
-    <t>Medium glucose -Ex4 vs low glucose -Ex40</t>
-  </si>
-  <si>
     <t>NAME of KEGG pathways</t>
+  </si>
+  <si>
+    <t>High glucose -Ex4 vs medium glucose -Ex4</t>
+  </si>
+  <si>
+    <t>Low  glucose +Ex4 vs low glucose -Ex4</t>
+  </si>
+  <si>
+    <t>Medium  glucose +Ex4 vs medium glucose -Ex4</t>
+  </si>
+  <si>
+    <t>Medium glucose -Ex4 vs low glucose -Ex4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -891,12 +486,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.33203125" customWidth="1"/>
     <col min="2" max="2" width="25.1640625" customWidth="1"/>
     <col min="3" max="3" width="47.1640625" customWidth="1"/>
     <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
@@ -905,15 +500,15 @@
     <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="16">
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>178</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -928,7 +523,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -951,9 +546,9 @@
         <v>0.73201024999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -974,9 +569,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
@@ -997,9 +592,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>30</v>
@@ -1020,9 +615,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
@@ -1043,9 +638,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
@@ -1066,9 +661,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
@@ -1089,9 +684,9 @@
         <v>0.97194510000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
@@ -1112,9 +707,9 @@
         <v>0.99407840000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
@@ -1135,9 +730,9 @@
         <v>0.9160585</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
@@ -1158,9 +753,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
@@ -1181,9 +776,9 @@
         <v>0.60291609999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
@@ -1204,9 +799,9 @@
         <v>0.94798552999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
@@ -1227,9 +822,9 @@
         <v>0.93856930000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
         <v>30</v>
@@ -1250,9 +845,9 @@
         <v>0.86676072999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
         <v>30</v>
@@ -1273,9 +868,9 @@
         <v>0.96009873999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
         <v>30</v>
@@ -1296,9 +891,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
@@ -1319,9 +914,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
         <v>30</v>
@@ -1342,9 +937,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
         <v>30</v>
@@ -1365,9 +960,9 @@
         <v>0.93614609999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
         <v>30</v>
@@ -1388,9 +983,9 @@
         <v>0.97557837000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
         <v>30</v>
@@ -1411,9 +1006,9 @@
         <v>0.96152269999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
         <v>30</v>
@@ -1434,9 +1029,9 @@
         <v>0.96806407000000005</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
         <v>30</v>
@@ -1457,12 +1052,12 @@
         <v>0.97669300000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -1480,12 +1075,12 @@
         <v>0.73685089999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
@@ -1503,12 +1098,12 @@
         <v>0.62148327000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
         <v>20</v>
@@ -1526,12 +1121,12 @@
         <v>0.42347994</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
         <v>22</v>
@@ -1549,12 +1144,12 @@
         <v>0.68226529999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
@@ -1572,12 +1167,12 @@
         <v>0.79292750000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
@@ -1595,12 +1190,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
         <v>21</v>
@@ -1618,12 +1213,12 @@
         <v>0.89082890000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C32" t="s">
         <v>8</v>
@@ -1641,12 +1236,12 @@
         <v>0.8971983</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C33" t="s">
         <v>10</v>
@@ -1664,12 +1259,12 @@
         <v>0.87032810000000005</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C34" t="s">
         <v>11</v>
@@ -1687,12 +1282,12 @@
         <v>0.78707839999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C35" t="s">
         <v>25</v>
@@ -1710,12 +1305,12 @@
         <v>0.91673020000000005</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C36" t="s">
         <v>28</v>
@@ -1733,12 +1328,12 @@
         <v>0.89546230000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
         <v>24</v>
@@ -1756,12 +1351,12 @@
         <v>0.90290475000000003</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C38" t="s">
         <v>13</v>
@@ -1779,12 +1374,12 @@
         <v>0.89734700000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C39" t="s">
         <v>16</v>
@@ -1802,12 +1397,12 @@
         <v>6.2849080000000002E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C40" t="s">
         <v>19</v>
@@ -1825,12 +1420,12 @@
         <v>8.4566063999999996E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C41" t="s">
         <v>26</v>
@@ -1848,12 +1443,12 @@
         <v>7.5822349999999997E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C42" t="s">
         <v>18</v>
@@ -1871,12 +1466,12 @@
         <v>9.4100459999999997E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
@@ -1894,12 +1489,12 @@
         <v>0.24942202999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C44" t="s">
         <v>27</v>
@@ -1917,12 +1512,12 @@
         <v>0.32160636999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C45" t="s">
         <v>12</v>
@@ -1940,12 +1535,12 @@
         <v>0.55495470000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C46" t="s">
         <v>29</v>
@@ -1963,12 +1558,12 @@
         <v>0.79897569999999996</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C47" t="s">
         <v>10</v>
@@ -1986,12 +1581,12 @@
         <v>0.39382764999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C48" t="s">
         <v>28</v>
@@ -2009,12 +1604,12 @@
         <v>0.31691560000000002</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>81</v>
+        <v>40</v>
       </c>
       <c r="B49" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C49" t="s">
         <v>8</v>
@@ -2032,12 +1627,12 @@
         <v>0.27727336000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="B50" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C50" t="s">
         <v>4</v>
@@ -2055,12 +1650,12 @@
         <v>0.22542867</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="B51" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C51" t="s">
         <v>20</v>
@@ -2078,12 +1673,12 @@
         <v>0.41763922999999997</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="B52" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C52" t="s">
         <v>22</v>
@@ -2101,12 +1696,12 @@
         <v>0.56388660000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="B53" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C53" t="s">
         <v>12</v>
@@ -2124,12 +1719,12 @@
         <v>0.50802343999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="B54" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C54" t="s">
         <v>9</v>
@@ -2147,12 +1742,12 @@
         <v>0.63599640000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="B55" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C55" t="s">
         <v>13</v>
@@ -2170,12 +1765,12 @@
         <v>0.64523923000000005</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="B56" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C56" t="s">
         <v>18</v>
@@ -2193,12 +1788,12 @@
         <v>0.66436189999999995</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C57" t="s">
         <v>24</v>
@@ -2216,12 +1811,12 @@
         <v>0.69952285000000003</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="B58" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C58" t="s">
         <v>21</v>
@@ -2239,12 +1834,12 @@
         <v>0.91719740000000005</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C59" t="s">
         <v>6</v>
@@ -2262,12 +1857,12 @@
         <v>0.91856369999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="B60" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C60" t="s">
         <v>29</v>
@@ -2285,12 +1880,12 @@
         <v>0.86662817000000003</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>93</v>
+        <v>40</v>
       </c>
       <c r="B61" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C61" t="s">
         <v>7</v>
@@ -2308,12 +1903,12 @@
         <v>0.82175180000000003</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="B62" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C62" t="s">
         <v>26</v>
@@ -2331,12 +1926,12 @@
         <v>0.81566554000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="B63" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C63" t="s">
         <v>23</v>
@@ -2354,12 +1949,12 @@
         <v>0.90239789999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="B64" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C64" t="s">
         <v>19</v>
@@ -2377,12 +1972,12 @@
         <v>7.2163100000000001E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="B65" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C65" t="s">
         <v>11</v>
@@ -2400,12 +1995,12 @@
         <v>0.58802049999999995</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="B66" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C66" t="s">
         <v>16</v>
@@ -2423,12 +2018,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="B67" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C67" t="s">
         <v>27</v>
@@ -2446,12 +2041,12 @@
         <v>0.87536579999999997</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="B68" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C68" t="s">
         <v>5</v>
@@ -2469,12 +2064,12 @@
         <v>0.70736359999999998</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>101</v>
+        <v>40</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="C69" t="s">
         <v>25</v>
@@ -2492,12 +2087,12 @@
         <v>0.94386183999999995</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>103</v>
+        <v>41</v>
       </c>
       <c r="B70" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C70" t="s">
         <v>21</v>
@@ -2515,12 +2110,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>104</v>
+        <v>41</v>
       </c>
       <c r="B71" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C71" t="s">
         <v>18</v>
@@ -2538,12 +2133,12 @@
         <v>0.90924490000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>105</v>
+        <v>41</v>
       </c>
       <c r="B72" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C72" t="s">
         <v>16</v>
@@ -2561,12 +2156,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>106</v>
+        <v>41</v>
       </c>
       <c r="B73" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C73" t="s">
         <v>15</v>
@@ -2584,12 +2179,12 @@
         <v>0.99266726000000005</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>107</v>
+        <v>41</v>
       </c>
       <c r="B74" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C74" t="s">
         <v>9</v>
@@ -2607,12 +2202,12 @@
         <v>0.82383649999999997</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="B75" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C75" t="s">
         <v>28</v>
@@ -2630,12 +2225,12 @@
         <v>0.68991329999999995</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>109</v>
+        <v>41</v>
       </c>
       <c r="B76" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C76" t="s">
         <v>27</v>
@@ -2653,12 +2248,12 @@
         <v>0.89137639999999996</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>110</v>
+        <v>41</v>
       </c>
       <c r="B77" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C77" t="s">
         <v>8</v>
@@ -2676,12 +2271,12 @@
         <v>0.85621239999999998</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>111</v>
+        <v>41</v>
       </c>
       <c r="B78" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C78" t="s">
         <v>7</v>
@@ -2699,12 +2294,12 @@
         <v>0.97145570000000003</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>112</v>
+        <v>41</v>
       </c>
       <c r="B79" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C79" t="s">
         <v>13</v>
@@ -2722,12 +2317,12 @@
         <v>0.87992035999999996</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>113</v>
+        <v>41</v>
       </c>
       <c r="B80" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C80" t="s">
         <v>11</v>
@@ -2745,12 +2340,12 @@
         <v>0.91331046999999999</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="B81" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C81" t="s">
         <v>14</v>
@@ -2768,12 +2363,12 @@
         <v>0.85949540000000002</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>115</v>
+        <v>41</v>
       </c>
       <c r="B82" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C82" t="s">
         <v>23</v>
@@ -2791,12 +2386,12 @@
         <v>0.94603055999999996</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>116</v>
+        <v>41</v>
       </c>
       <c r="B83" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C83" t="s">
         <v>24</v>
@@ -2814,12 +2409,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="B84" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C84" t="s">
         <v>10</v>
@@ -2837,12 +2432,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>118</v>
+        <v>41</v>
       </c>
       <c r="B85" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C85" t="s">
         <v>20</v>
@@ -2860,12 +2455,12 @@
         <v>0.97060584999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>119</v>
+        <v>41</v>
       </c>
       <c r="B86" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C86" t="s">
         <v>4</v>
@@ -2883,12 +2478,12 @@
         <v>1.3333333E-4</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>120</v>
+        <v>41</v>
       </c>
       <c r="B87" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C87" t="s">
         <v>22</v>
@@ -2906,12 +2501,12 @@
         <v>0.11172893</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>121</v>
+        <v>41</v>
       </c>
       <c r="B88" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C88" t="s">
         <v>19</v>
@@ -2929,12 +2524,12 @@
         <v>0.86002520000000005</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>122</v>
+        <v>41</v>
       </c>
       <c r="B89" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C89" t="s">
         <v>6</v>
@@ -2952,12 +2547,12 @@
         <v>0.75728609999999996</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>123</v>
+        <v>41</v>
       </c>
       <c r="B90" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C90" t="s">
         <v>29</v>
@@ -2975,12 +2570,12 @@
         <v>0.67859393000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>124</v>
+        <v>41</v>
       </c>
       <c r="B91" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C91" t="s">
         <v>25</v>
@@ -2998,12 +2593,12 @@
         <v>0.64713584999999996</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7">
       <c r="A92" t="s">
-        <v>125</v>
+        <v>41</v>
       </c>
       <c r="B92" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C92" t="s">
         <v>12</v>
@@ -3021,12 +2616,12 @@
         <v>0.57760893999999996</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7">
       <c r="A93" t="s">
-        <v>126</v>
+        <v>41</v>
       </c>
       <c r="B93" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="C93" t="s">
         <v>26</v>
@@ -3044,12 +2639,12 @@
         <v>0.87353826000000001</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>128</v>
+        <v>42</v>
       </c>
       <c r="B94" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C94" t="s">
         <v>5</v>
@@ -3067,12 +2662,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7">
       <c r="A95" t="s">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="B95" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C95" t="s">
         <v>22</v>
@@ -3090,12 +2685,12 @@
         <v>0.86297124999999997</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7">
       <c r="A96" t="s">
-        <v>130</v>
+        <v>42</v>
       </c>
       <c r="B96" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C96" t="s">
         <v>19</v>
@@ -3113,12 +2708,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>131</v>
+        <v>42</v>
       </c>
       <c r="B97" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C97" t="s">
         <v>18</v>
@@ -3136,12 +2731,12 @@
         <v>0.92998630000000004</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>132</v>
+        <v>42</v>
       </c>
       <c r="B98" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C98" t="s">
         <v>20</v>
@@ -3159,12 +2754,12 @@
         <v>0.81029015999999998</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>133</v>
+        <v>42</v>
       </c>
       <c r="B99" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C99" t="s">
         <v>28</v>
@@ -3182,12 +2777,12 @@
         <v>0.95199363999999997</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>134</v>
+        <v>42</v>
       </c>
       <c r="B100" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C100" t="s">
         <v>6</v>
@@ -3205,12 +2800,12 @@
         <v>0.86449160000000003</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7">
       <c r="A101" t="s">
-        <v>135</v>
+        <v>42</v>
       </c>
       <c r="B101" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C101" t="s">
         <v>25</v>
@@ -3228,12 +2823,12 @@
         <v>0.88187634999999998</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7">
       <c r="A102" t="s">
-        <v>136</v>
+        <v>42</v>
       </c>
       <c r="B102" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C102" t="s">
         <v>15</v>
@@ -3251,12 +2846,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7">
       <c r="A103" t="s">
-        <v>137</v>
+        <v>42</v>
       </c>
       <c r="B103" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C103" t="s">
         <v>14</v>
@@ -3274,12 +2869,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7">
       <c r="A104" t="s">
-        <v>138</v>
+        <v>42</v>
       </c>
       <c r="B104" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C104" t="s">
         <v>12</v>
@@ -3297,12 +2892,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7">
       <c r="A105" t="s">
-        <v>139</v>
+        <v>42</v>
       </c>
       <c r="B105" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C105" t="s">
         <v>4</v>
@@ -3320,12 +2915,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7">
       <c r="A106" t="s">
-        <v>140</v>
+        <v>42</v>
       </c>
       <c r="B106" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C106" t="s">
         <v>24</v>
@@ -3343,12 +2938,12 @@
         <v>0.98001015000000002</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7">
       <c r="A107" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="B107" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C107" t="s">
         <v>10</v>
@@ -3366,12 +2961,12 @@
         <v>0.91042566000000003</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7">
       <c r="A108" t="s">
-        <v>142</v>
+        <v>42</v>
       </c>
       <c r="B108" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C108" t="s">
         <v>11</v>
@@ -3389,12 +2984,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7">
       <c r="A109" t="s">
-        <v>143</v>
+        <v>42</v>
       </c>
       <c r="B109" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C109" t="s">
         <v>8</v>
@@ -3412,12 +3007,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7">
       <c r="A110" t="s">
-        <v>144</v>
+        <v>42</v>
       </c>
       <c r="B110" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C110" t="s">
         <v>23</v>
@@ -3435,12 +3030,12 @@
         <v>0.99800705999999995</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7">
       <c r="A111" t="s">
-        <v>145</v>
+        <v>42</v>
       </c>
       <c r="B111" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C111" t="s">
         <v>21</v>
@@ -3458,12 +3053,12 @@
         <v>0.99421256999999996</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>146</v>
+        <v>42</v>
       </c>
       <c r="B112" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C112" t="s">
         <v>16</v>
@@ -3481,12 +3076,12 @@
         <v>0.91537100000000005</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7">
       <c r="A113" t="s">
-        <v>147</v>
+        <v>42</v>
       </c>
       <c r="B113" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C113" t="s">
         <v>7</v>
@@ -3504,12 +3099,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7">
       <c r="A114" t="s">
-        <v>148</v>
+        <v>42</v>
       </c>
       <c r="B114" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C114" t="s">
         <v>26</v>
@@ -3527,12 +3122,12 @@
         <v>0.94818440000000004</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7">
       <c r="A115" t="s">
-        <v>149</v>
+        <v>42</v>
       </c>
       <c r="B115" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C115" t="s">
         <v>29</v>
@@ -3550,12 +3145,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7">
       <c r="A116" t="s">
-        <v>150</v>
+        <v>42</v>
       </c>
       <c r="B116" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C116" t="s">
         <v>13</v>
@@ -3573,12 +3168,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7">
       <c r="A117" t="s">
-        <v>151</v>
+        <v>42</v>
       </c>
       <c r="B117" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C117" t="s">
         <v>27</v>
@@ -3596,12 +3191,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7">
       <c r="A118" t="s">
-        <v>152</v>
+        <v>42</v>
       </c>
       <c r="B118" t="s">
-        <v>127</v>
+        <v>37</v>
       </c>
       <c r="C118" t="s">
         <v>9</v>
@@ -3619,12 +3214,12 @@
         <v>0.99680877000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7">
       <c r="A119" t="s">
-        <v>153</v>
+        <v>43</v>
       </c>
       <c r="B119" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C119" t="s">
         <v>9</v>
@@ -3642,12 +3237,12 @@
         <v>0.69766499999999998</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7">
       <c r="A120" t="s">
-        <v>155</v>
+        <v>43</v>
       </c>
       <c r="B120" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C120" t="s">
         <v>20</v>
@@ -3665,12 +3260,12 @@
         <v>0.9873208</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7">
       <c r="A121" t="s">
-        <v>156</v>
+        <v>43</v>
       </c>
       <c r="B121" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C121" t="s">
         <v>11</v>
@@ -3688,12 +3283,12 @@
         <v>0.75320469999999995</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7">
       <c r="A122" t="s">
-        <v>157</v>
+        <v>43</v>
       </c>
       <c r="B122" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C122" t="s">
         <v>4</v>
@@ -3711,12 +3306,12 @@
         <v>0.88268113000000004</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7">
       <c r="A123" t="s">
-        <v>158</v>
+        <v>43</v>
       </c>
       <c r="B123" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C123" t="s">
         <v>14</v>
@@ -3734,12 +3329,12 @@
         <v>0.79150960000000004</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7">
       <c r="A124" t="s">
-        <v>159</v>
+        <v>43</v>
       </c>
       <c r="B124" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C124" t="s">
         <v>23</v>
@@ -3757,12 +3352,12 @@
         <v>0.88638406999999997</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7">
       <c r="A125" t="s">
-        <v>160</v>
+        <v>43</v>
       </c>
       <c r="B125" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C125" t="s">
         <v>22</v>
@@ -3780,12 +3375,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7">
       <c r="A126" t="s">
-        <v>161</v>
+        <v>43</v>
       </c>
       <c r="B126" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C126" t="s">
         <v>6</v>
@@ -3803,12 +3398,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7">
       <c r="A127" t="s">
-        <v>162</v>
+        <v>43</v>
       </c>
       <c r="B127" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C127" t="s">
         <v>21</v>
@@ -3826,12 +3421,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7">
       <c r="A128" t="s">
-        <v>163</v>
+        <v>43</v>
       </c>
       <c r="B128" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C128" t="s">
         <v>25</v>
@@ -3849,12 +3444,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7">
       <c r="A129" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="B129" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C129" t="s">
         <v>28</v>
@@ -3872,12 +3467,12 @@
         <v>0.96554434</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7">
       <c r="A130" t="s">
-        <v>165</v>
+        <v>43</v>
       </c>
       <c r="B130" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C130" t="s">
         <v>24</v>
@@ -3895,12 +3490,12 @@
         <v>0.99247633999999996</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7">
       <c r="A131" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
       <c r="B131" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C131" t="s">
         <v>10</v>
@@ -3918,12 +3513,12 @@
         <v>0.92603457</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7">
       <c r="A132" t="s">
-        <v>167</v>
+        <v>43</v>
       </c>
       <c r="B132" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C132" t="s">
         <v>16</v>
@@ -3941,12 +3536,12 @@
         <v>7.7640905999999996E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7">
       <c r="A133" t="s">
-        <v>168</v>
+        <v>43</v>
       </c>
       <c r="B133" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C133" t="s">
         <v>26</v>
@@ -3964,12 +3559,12 @@
         <v>3.9384021999999998E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7">
       <c r="A134" t="s">
-        <v>169</v>
+        <v>43</v>
       </c>
       <c r="B134" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C134" t="s">
         <v>19</v>
@@ -3987,12 +3582,12 @@
         <v>0.10406183500000001</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7">
       <c r="A135" t="s">
-        <v>170</v>
+        <v>43</v>
       </c>
       <c r="B135" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C135" t="s">
         <v>18</v>
@@ -4010,12 +3605,12 @@
         <v>0.13931154000000001</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7">
       <c r="A136" t="s">
-        <v>171</v>
+        <v>43</v>
       </c>
       <c r="B136" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C136" t="s">
         <v>7</v>
@@ -4033,12 +3628,12 @@
         <v>0.16711709</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7">
       <c r="A137" t="s">
-        <v>172</v>
+        <v>43</v>
       </c>
       <c r="B137" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C137" t="s">
         <v>12</v>
@@ -4056,12 +3651,12 @@
         <v>0.36953272999999998</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7">
       <c r="A138" t="s">
-        <v>173</v>
+        <v>43</v>
       </c>
       <c r="B138" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C138" t="s">
         <v>15</v>
@@ -4079,12 +3674,12 @@
         <v>0.85207087000000004</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7">
       <c r="A139" t="s">
-        <v>174</v>
+        <v>43</v>
       </c>
       <c r="B139" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C139" t="s">
         <v>13</v>
@@ -4102,12 +3697,12 @@
         <v>0.83308919999999997</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7">
       <c r="A140" t="s">
-        <v>175</v>
+        <v>43</v>
       </c>
       <c r="B140" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C140" t="s">
         <v>29</v>
@@ -4125,12 +3720,12 @@
         <v>0.75139296</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7">
       <c r="A141" t="s">
-        <v>176</v>
+        <v>43</v>
       </c>
       <c r="B141" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C141" t="s">
         <v>27</v>
@@ -4148,12 +3743,12 @@
         <v>0.84058314999999995</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7">
       <c r="A142" t="s">
-        <v>177</v>
+        <v>43</v>
       </c>
       <c r="B142" t="s">
-        <v>154</v>
+        <v>38</v>
       </c>
       <c r="C142" t="s">
         <v>8</v>
@@ -4171,64 +3766,64 @@
         <v>0.85527783999999996</v>
       </c>
     </row>
-    <row r="168" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="6:6">
       <c r="F168" s="1"/>
     </row>
-    <row r="215" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="215" spans="6:7">
       <c r="G215" s="1"/>
     </row>
-    <row r="217" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="217" spans="6:7">
       <c r="F217" s="1"/>
     </row>
-    <row r="218" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="218" spans="6:7">
       <c r="F218" s="1"/>
     </row>
-    <row r="219" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="219" spans="6:7">
       <c r="F219" s="1"/>
     </row>
-    <row r="251" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="251" spans="6:7">
       <c r="G251" s="1"/>
     </row>
-    <row r="253" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="253" spans="6:7">
       <c r="F253" s="1"/>
     </row>
-    <row r="301" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="301" spans="6:6">
       <c r="F301" s="1"/>
     </row>
-    <row r="337" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="337" spans="6:6">
       <c r="F337" s="1"/>
     </row>
-    <row r="384" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="384" spans="7:7">
       <c r="G384" s="1"/>
     </row>
-    <row r="417" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="417" spans="6:6">
       <c r="F417" s="1"/>
     </row>
-    <row r="443" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="443" spans="7:7">
       <c r="G443" s="1"/>
     </row>
-    <row r="444" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="444" spans="7:7">
       <c r="G444" s="1"/>
     </row>
-    <row r="445" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="445" spans="7:7">
       <c r="G445" s="1"/>
     </row>
-    <row r="446" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="446" spans="7:7">
       <c r="G446" s="1"/>
     </row>
-    <row r="447" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="447" spans="7:7">
       <c r="G447" s="1"/>
     </row>
-    <row r="448" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="448" spans="7:7">
       <c r="G448" s="1"/>
     </row>
-    <row r="450" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="450" spans="6:6">
       <c r="F450" s="1"/>
     </row>
-    <row r="451" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="451" spans="6:6">
       <c r="F451" s="1"/>
     </row>
-    <row r="452" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="452" spans="6:6">
       <c r="F452" s="1"/>
     </row>
   </sheetData>

</xml_diff>